<commit_message>
Fixed data after netsings changed.
</commit_message>
<xml_diff>
--- a/Articles/Presentation_ESEE_2015/Other results/Paul and Joao summary/PB_JS_Summary_Results Graphs and Table_PB_25_06_15.xlsx
+++ b/Articles/Presentation_ESEE_2015/Other results/Paul and Joao summary/PB_JS_Summary_Results Graphs and Table_PB_25_06_15.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7760" tabRatio="803" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7760" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Results Table" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,6 +623,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1098,9 +1114,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1510,6 +1536,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1570,34 +1622,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="12">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1649,7 +1685,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1667,7 +1702,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.98</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1870,10 +1905,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5</c:v>
+                  <c:v>0.509524</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.720815</c:v>
+                  <c:v>0.009391</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.0</c:v>
@@ -1894,7 +1929,7 @@
                   <c:v>0.66516</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.977066034005536</c:v>
+                  <c:v>1.74712</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.017991</c:v>
@@ -1903,10 +1938,10 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.5</c:v>
+                  <c:v>0.509524</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.720815</c:v>
+                  <c:v>0.009391</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.611818</c:v>
@@ -2205,10 +2240,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.009391</c:v>
+                  <c:v>0.720815</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0014357</c:v>
+                  <c:v>0.014357</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0.0</c:v>
@@ -2220,10 +2255,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.009391</c:v>
+                  <c:v>0.720815</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0014357</c:v>
+                  <c:v>0.014357</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00%">
                   <c:v>0.145</c:v>
@@ -2510,7 +2545,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="68"/>
                 <c:pt idx="0">
-                  <c:v>0.00941041846248819</c:v>
+                  <c:v>0.013645</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.017595</c:v>
@@ -2519,10 +2554,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.068505</c:v>
+                  <c:v>0.465188</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.109753</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00%">
                   <c:v>0.355</c:v>
@@ -2821,7 +2856,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0</c:v>
+                  <c:v>0.611994</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00%">
                   <c:v>0.345</c:v>
@@ -3108,13 +3143,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="68"/>
                 <c:pt idx="1">
-                  <c:v>0.186382867686802</c:v>
+                  <c:v>0.186281</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.103338</c:v>
+                  <c:v>1.340508</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.190138</c:v>
@@ -3218,11 +3253,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2136058312"/>
-        <c:axId val="2136061432"/>
+        <c:axId val="2127858056"/>
+        <c:axId val="2127854920"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2136058312"/>
+        <c:axId val="2127858056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3232,7 +3267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136061432"/>
+        <c:crossAx val="2127854920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3242,7 +3277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136061432"/>
+        <c:axId val="2127854920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3266,21 +3301,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136058312"/>
+        <c:crossAx val="2127858056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3857,11 +3890,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2139108056"/>
-        <c:axId val="2139111576"/>
+        <c:axId val="2126924040"/>
+        <c:axId val="2126927528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2139108056"/>
+        <c:axId val="2126924040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3904,7 +3937,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139111576"/>
+        <c:crossAx val="2126927528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3912,7 +3945,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2139111576"/>
+        <c:axId val="2126927528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3963,7 +3996,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139108056"/>
+        <c:crossAx val="2126924040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4129,11 +4162,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2142396136"/>
-        <c:axId val="2144902664"/>
+        <c:axId val="2126864392"/>
+        <c:axId val="2126867896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142396136"/>
+        <c:axId val="2126864392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4176,7 +4209,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144902664"/>
+        <c:crossAx val="2126867896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4184,7 +4217,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144902664"/>
+        <c:axId val="2126867896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4235,7 +4268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142396136"/>
+        <c:crossAx val="2126864392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5312,11 +5345,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2142265368"/>
-        <c:axId val="2142268872"/>
+        <c:axId val="2126598216"/>
+        <c:axId val="2126601704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142265368"/>
+        <c:axId val="2126598216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5359,7 +5392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142268872"/>
+        <c:crossAx val="2126601704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5367,7 +5400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142268872"/>
+        <c:axId val="2126601704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5418,7 +5451,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142265368"/>
+        <c:crossAx val="2126598216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5581,11 +5614,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2142301592"/>
-        <c:axId val="2142305096"/>
+        <c:axId val="2126517464"/>
+        <c:axId val="2126520968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142301592"/>
+        <c:axId val="2126517464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5628,7 +5661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142305096"/>
+        <c:crossAx val="2126520968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5636,7 +5669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142305096"/>
+        <c:axId val="2126520968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5687,7 +5720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142301592"/>
+        <c:crossAx val="2126517464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5843,7 +5876,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.031238865</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.031238254</c:v>
@@ -5930,7 +5963,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.031238865</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.76625336518544E-22</c:v>
@@ -6023,7 +6056,7 @@
                   <c:v>4.4164299884406E-12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00301710034676472</c:v>
+                  <c:v>0.00315656962251</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -6144,11 +6177,11 @@
         </c:dLbls>
         <c:gapWidth val="300"/>
         <c:overlap val="100"/>
-        <c:axId val="2143584376"/>
-        <c:axId val="2135992968"/>
+        <c:axId val="2127811592"/>
+        <c:axId val="2127808456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143584376"/>
+        <c:axId val="2127811592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6157,7 +6190,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135992968"/>
+        <c:crossAx val="2127808456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6165,7 +6198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135992968"/>
+        <c:axId val="2127808456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.04"/>
@@ -6176,7 +6209,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143584376"/>
+        <c:crossAx val="2127811592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6380,10 +6413,10 @@
                   <c:v>0.269081</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.4942</c:v>
+                  <c:v>-0.427629470213838</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>1.977066034005536</c:v>
+                  <c:v>1.74712</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>11.73690646015896</c:v>
@@ -6631,7 +6664,7 @@
                   <c:v>3.06195E-11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.09287188</c:v>
+                  <c:v>0.097165</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.000">
                   <c:v>54.58334722917014</c:v>
@@ -6874,25 +6907,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.4395963</c:v>
+                  <c:v>0.445423</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5604037</c:v>
+                  <c:v>0.554757</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>8.024692E-13</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>105.4849323820679</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.009391</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.38731852139592</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6" formatCode="0.000">
                   <c:v>0.720815</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>105.4849323820679</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.000">
-                  <c:v>0.009391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7127,13 +7160,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.4203956</c:v>
+                  <c:v>0.426684</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4171007</c:v>
+                  <c:v>0.421804</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1625037</c:v>
+                  <c:v>0.151512</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.634472996871619</c:v>
@@ -7142,10 +7175,10 @@
                   <c:v>0.611818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>695.5243435258062</c:v>
+                  <c:v>68.65243435258063</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.000">
-                  <c:v>0.0014357</c:v>
+                  <c:v>0.014357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7367,11 +7400,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2142683864"/>
-        <c:axId val="2140167688"/>
+        <c:axId val="2124951464"/>
+        <c:axId val="2124934824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142683864"/>
+        <c:axId val="2124951464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7414,7 +7447,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140167688"/>
+        <c:crossAx val="2124934824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7422,7 +7455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140167688"/>
+        <c:axId val="2124934824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7473,7 +7506,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142683864"/>
+        <c:crossAx val="2124951464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7632,10 +7665,10 @@
                   <c:v>0.001651163</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>0.0144077</c:v>
+                  <c:v>0.013857</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.000">
-                  <c:v>0.006991347</c:v>
+                  <c:v>0.007103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7651,11 +7684,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2140291240"/>
-        <c:axId val="2140294744"/>
+        <c:axId val="2124815528"/>
+        <c:axId val="2124819032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140291240"/>
+        <c:axId val="2124815528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7698,7 +7731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140294744"/>
+        <c:crossAx val="2124819032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7706,7 +7739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140294744"/>
+        <c:axId val="2124819032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7757,7 +7790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140291240"/>
+        <c:crossAx val="2124815528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7958,10 +7991,10 @@
                   <c:v>4.774411E-16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.2652</c:v>
+                  <c:v>72.28691828508611</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>0.00941041846248819</c:v>
+                  <c:v>0.013645</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.506975659773319</c:v>
@@ -8452,19 +8485,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.791632</c:v>
+                  <c:v>0.570049</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.002742913</c:v>
+                  <c:v>0.134387</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.205625</c:v>
+                  <c:v>0.295564</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.59747463688782</c:v>
+                  <c:v>1.149668521114044</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.068505</c:v>
+                  <c:v>0.465188</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-1.0</c:v>
@@ -8701,25 +8734,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.7379566</c:v>
+                  <c:v>0.469167</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.03470879</c:v>
+                  <c:v>0.144017</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2273346</c:v>
+                  <c:v>0.386817</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.111368254170729</c:v>
+                  <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>0.109753</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-1.0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.000">
-                  <c:v>0.0</c:v>
+                  <c:v>0.611994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8919,25 +8952,25 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.003973582476072</c:v>
+                  <c:v>0.003871393838</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.007971783551066</c:v>
+                  <c:v>0.007921884795</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0071503628831268</c:v>
+                  <c:v>0.007209679548</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0141556952488238</c:v>
+                  <c:v>0.013859680032</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00036656176536</c:v>
+                  <c:v>0.000335164764</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.000945541093440001</c:v>
+                  <c:v>0.00214908473</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00421673958849</c:v>
+                  <c:v>0.004517925489</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.002679101797716</c:v>
@@ -9006,25 +9039,25 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.008179271988228</c:v>
+                  <c:v>0.008129282564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0003749420510629</c:v>
+                  <c:v>0.002431727045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0070943210723571</c:v>
+                  <c:v>0.007127222188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0081931417511762</c:v>
+                  <c:v>0.008184319968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00105006082671</c:v>
+                  <c:v>0.000973004273999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.27619014546E-6</c:v>
+                  <c:v>0.00050663899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00537556041151</c:v>
+                  <c:v>0.005626900251</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.00343866982284</c:v>
@@ -9093,25 +9126,25 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.000760706181378</c:v>
+                  <c:v>0.000661323598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.002455784289846</c:v>
+                  <c:v>0.006531405045</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0027639690445161</c:v>
+                  <c:v>0.002560098264</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.032750353565E-5</c:v>
+                  <c:v>9.83227999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0002456026125</c:v>
+                  <c:v>0.00111427628</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.69752530716E-15</c:v>
+                  <c:v>8.1394450956E-15</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -9180,25 +9213,25 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.01108644</c:v>
+                  <c:v>0.011338</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01319749</c:v>
+                  <c:v>0.007115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.006991347</c:v>
+                  <c:v>0.007103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.001651163</c:v>
+                  <c:v>0.001956</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.02257305</c:v>
+                  <c:v>0.022682</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.02280558</c:v>
+                  <c:v>0.02023</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0144077</c:v>
+                  <c:v>0.013857</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.01788063</c:v>
@@ -9220,11 +9253,11 @@
         </c:dLbls>
         <c:gapWidth val="300"/>
         <c:overlap val="100"/>
-        <c:axId val="2143675864"/>
-        <c:axId val="2143793352"/>
+        <c:axId val="2127766520"/>
+        <c:axId val="2127763384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143675864"/>
+        <c:axId val="2127766520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9233,7 +9266,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143793352"/>
+        <c:crossAx val="2127763384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9241,7 +9274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143793352"/>
+        <c:axId val="2127763384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.04"/>
@@ -9252,7 +9285,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143675864"/>
+        <c:crossAx val="2127766520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.01"/>
@@ -9420,11 +9453,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2142732680"/>
-        <c:axId val="2142712248"/>
+        <c:axId val="2124721464"/>
+        <c:axId val="2124681592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142732680"/>
+        <c:axId val="2124721464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9467,7 +9500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142712248"/>
+        <c:crossAx val="2124681592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9475,7 +9508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142712248"/>
+        <c:axId val="2124681592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9526,7 +9559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142732680"/>
+        <c:crossAx val="2124721464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9677,10 +9710,10 @@
                   <c:v>0.001651163</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>0.02280558</c:v>
+                  <c:v>0.02023</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.000">
-                  <c:v>0.01319749</c:v>
+                  <c:v>0.007115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9696,11 +9729,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2103473720"/>
-        <c:axId val="2103449336"/>
+        <c:axId val="2133886808"/>
+        <c:axId val="2134872344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2103473720"/>
+        <c:axId val="2133886808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9743,7 +9776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103449336"/>
+        <c:crossAx val="2134872344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9751,7 +9784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103449336"/>
+        <c:axId val="2134872344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9802,7 +9835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103473720"/>
+        <c:crossAx val="2133886808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9998,10 +10031,10 @@
                   <c:v>1.169187E-13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3653</c:v>
+                  <c:v>4.368234012057053</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.000">
-                  <c:v>0.186382867686802</c:v>
+                  <c:v>0.186281</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>191.5669170036588</c:v>
@@ -10238,19 +10271,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.762917E-14</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.000">
-                  <c:v>4.044899606497831</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.000">
-                  <c:v>0.19822</c:v>
+                <c:pt idx="3" formatCode="0.000">
+                  <c:v>57.77858108505261</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000">
+                  <c:v>0.017013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10486,25 +10519,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.2568848</c:v>
+                  <c:v>0.254298</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7358778</c:v>
+                  <c:v>0.738243</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.007237467</c:v>
+                  <c:v>0.00746</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>-0.254014149859605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.340508</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>8.676982329830264</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6" formatCode="0.000">
                   <c:v>0.103338</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.254014149859605</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.000">
-                  <c:v>1.340508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10740,13 +10773,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.3077062</c:v>
+                  <c:v>0.305749</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6333863</c:v>
+                  <c:v>0.642022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05890755</c:v>
+                  <c:v>0.052229</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.259337954538283</c:v>
@@ -10972,11 +11005,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2135025400"/>
-        <c:axId val="2135030968"/>
+        <c:axId val="2134867896"/>
+        <c:axId val="2134732584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135025400"/>
+        <c:axId val="2134867896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11019,7 +11052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135030968"/>
+        <c:crossAx val="2134732584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11027,7 +11060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135030968"/>
+        <c:axId val="2134732584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11078,7 +11111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135025400"/>
+        <c:crossAx val="2134867896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11229,10 +11262,10 @@
                   <c:v>0.001651163</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000">
-                  <c:v>0.02257305</c:v>
+                  <c:v>0.022682</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.000">
-                  <c:v>0.01108644</c:v>
+                  <c:v>0.011338</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11248,11 +11281,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2135062664"/>
-        <c:axId val="2135066168"/>
+        <c:axId val="2134663416"/>
+        <c:axId val="2134666904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135062664"/>
+        <c:axId val="2134663416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11295,7 +11328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135066168"/>
+        <c:crossAx val="2134666904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11303,7 +11336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135066168"/>
+        <c:axId val="2134666904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11354,7 +11387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2135062664"/>
+        <c:crossAx val="2134663416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -33168,7 +33201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -33181,8 +33214,11 @@
   </sheetPr>
   <dimension ref="B2:AF34"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6400" ySplit="2580" topLeftCell="R8" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -33251,91 +33287,91 @@
       <c r="Y5" s="11"/>
     </row>
     <row r="6" spans="2:32">
-      <c r="B6" s="153" t="s">
+      <c r="B6" s="163" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="154" t="s">
+      <c r="C6" s="164" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="155"/>
-      <c r="E6" s="167" t="s">
+      <c r="D6" s="165"/>
+      <c r="E6" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="168"/>
-      <c r="G6" s="168"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="168"/>
-      <c r="J6" s="168"/>
-      <c r="K6" s="168"/>
-      <c r="L6" s="168"/>
-      <c r="M6" s="168"/>
-      <c r="N6" s="168"/>
-      <c r="O6" s="168"/>
-      <c r="P6" s="169"/>
-      <c r="Q6" s="167" t="s">
+      <c r="F6" s="148"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+      <c r="J6" s="148"/>
+      <c r="K6" s="148"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
+      <c r="N6" s="148"/>
+      <c r="O6" s="148"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="168"/>
-      <c r="S6" s="168"/>
-      <c r="T6" s="168"/>
-      <c r="U6" s="168"/>
-      <c r="V6" s="168"/>
-      <c r="W6" s="168"/>
-      <c r="X6" s="168"/>
-      <c r="Y6" s="168"/>
-      <c r="Z6" s="168"/>
-      <c r="AA6" s="168"/>
-      <c r="AB6" s="168"/>
-      <c r="AC6" s="168"/>
-      <c r="AD6" s="168"/>
-      <c r="AE6" s="168"/>
-      <c r="AF6" s="169"/>
+      <c r="R6" s="148"/>
+      <c r="S6" s="148"/>
+      <c r="T6" s="148"/>
+      <c r="U6" s="148"/>
+      <c r="V6" s="148"/>
+      <c r="W6" s="148"/>
+      <c r="X6" s="148"/>
+      <c r="Y6" s="148"/>
+      <c r="Z6" s="148"/>
+      <c r="AA6" s="148"/>
+      <c r="AB6" s="148"/>
+      <c r="AC6" s="148"/>
+      <c r="AD6" s="148"/>
+      <c r="AE6" s="148"/>
+      <c r="AF6" s="149"/>
     </row>
     <row r="7" spans="2:32">
-      <c r="B7" s="149"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="157"/>
-      <c r="E7" s="170" t="s">
+      <c r="B7" s="159"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="171"/>
-      <c r="G7" s="171"/>
-      <c r="H7" s="171"/>
+      <c r="F7" s="151"/>
+      <c r="G7" s="151"/>
+      <c r="H7" s="151"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
-      <c r="K7" s="172" t="s">
+      <c r="K7" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="171"/>
-      <c r="M7" s="171"/>
-      <c r="N7" s="171"/>
-      <c r="O7" s="171"/>
-      <c r="P7" s="173"/>
-      <c r="Q7" s="170" t="s">
+      <c r="L7" s="151"/>
+      <c r="M7" s="151"/>
+      <c r="N7" s="151"/>
+      <c r="O7" s="151"/>
+      <c r="P7" s="153"/>
+      <c r="Q7" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="R7" s="171"/>
-      <c r="S7" s="171"/>
-      <c r="T7" s="171"/>
-      <c r="U7" s="171"/>
-      <c r="V7" s="171"/>
-      <c r="W7" s="171"/>
-      <c r="X7" s="176"/>
-      <c r="Y7" s="172" t="s">
+      <c r="R7" s="151"/>
+      <c r="S7" s="151"/>
+      <c r="T7" s="151"/>
+      <c r="U7" s="151"/>
+      <c r="V7" s="151"/>
+      <c r="W7" s="151"/>
+      <c r="X7" s="156"/>
+      <c r="Y7" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="Z7" s="171"/>
-      <c r="AA7" s="171"/>
-      <c r="AB7" s="171"/>
-      <c r="AC7" s="171"/>
-      <c r="AD7" s="171"/>
-      <c r="AE7" s="171"/>
-      <c r="AF7" s="173"/>
+      <c r="Z7" s="151"/>
+      <c r="AA7" s="151"/>
+      <c r="AB7" s="151"/>
+      <c r="AC7" s="151"/>
+      <c r="AD7" s="151"/>
+      <c r="AE7" s="151"/>
+      <c r="AF7" s="153"/>
     </row>
     <row r="8" spans="2:32" ht="17" thickBot="1">
-      <c r="B8" s="150"/>
-      <c r="C8" s="158"/>
-      <c r="D8" s="159"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="169"/>
       <c r="E8" s="8" t="s">
         <v>0</v>
       </c>
@@ -33463,13 +33499,13 @@
       <c r="AF9" s="20"/>
     </row>
     <row r="10" spans="2:32" ht="15" thickBot="1">
-      <c r="B10" s="164" t="s">
+      <c r="B10" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="160" t="s">
+      <c r="C10" s="170" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="161"/>
+      <c r="D10" s="171"/>
       <c r="E10" s="32">
         <v>1.6080000000000001E-2</v>
       </c>
@@ -33511,11 +33547,11 @@
       <c r="AF10" s="116"/>
     </row>
     <row r="11" spans="2:32" ht="15" thickBot="1">
-      <c r="B11" s="165"/>
-      <c r="C11" s="160" t="s">
+      <c r="B11" s="175"/>
+      <c r="C11" s="170" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="161"/>
+      <c r="D11" s="171"/>
       <c r="E11" s="32">
         <v>-5.5982899999999997E-3</v>
       </c>
@@ -33596,7 +33632,7 @@
       </c>
     </row>
     <row r="12" spans="2:32" ht="15" thickBot="1">
-      <c r="B12" s="165"/>
+      <c r="B12" s="175"/>
       <c r="C12" s="22"/>
       <c r="D12" s="23"/>
       <c r="E12" s="34" t="s">
@@ -33637,8 +33673,8 @@
       <c r="AF12" s="56"/>
     </row>
     <row r="13" spans="2:32" ht="15" thickBot="1">
-      <c r="B13" s="165"/>
-      <c r="C13" s="162" t="s">
+      <c r="B13" s="175"/>
+      <c r="C13" s="172" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="13" t="s">
@@ -33693,8 +33729,8 @@
       <c r="AF13" s="60"/>
     </row>
     <row r="14" spans="2:32" ht="15" thickBot="1">
-      <c r="B14" s="165"/>
-      <c r="C14" s="163"/>
+      <c r="B14" s="175"/>
+      <c r="C14" s="173"/>
       <c r="D14" s="13" t="s">
         <v>67</v>
       </c>
@@ -33759,8 +33795,8 @@
       <c r="AF14" s="60"/>
     </row>
     <row r="15" spans="2:32">
-      <c r="B15" s="165"/>
-      <c r="C15" s="163"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="173"/>
       <c r="D15" s="3" t="s">
         <v>68</v>
       </c>
@@ -33800,12 +33836,12 @@
       <c r="T15" s="65">
         <v>0.26908100000000001</v>
       </c>
-      <c r="U15" s="65">
-        <v>-0.49419999999999997</v>
+      <c r="U15" s="57">
+        <f>(1-V15)/V15</f>
+        <v>-0.42762947021383763</v>
       </c>
       <c r="V15" s="84">
-        <f>1/(1+U15)</f>
-        <v>1.9770660340055357</v>
+        <v>1.74712</v>
       </c>
       <c r="W15" s="57">
         <f>(1-X15)/X15</f>
@@ -33825,7 +33861,7 @@
         <v>3.0619499999999996E-11</v>
       </c>
       <c r="AB15" s="65">
-        <v>9.2871880000000004E-2</v>
+        <v>9.7165000000000001E-2</v>
       </c>
       <c r="AC15" s="90">
         <f>(1-AD15)/AD15</f>
@@ -33842,8 +33878,8 @@
       </c>
     </row>
     <row r="16" spans="2:32">
-      <c r="B16" s="165"/>
-      <c r="C16" s="163"/>
+      <c r="B16" s="175"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="3" t="s">
         <v>69</v>
       </c>
@@ -33878,11 +33914,11 @@
         <v>4.7744109999999992E-16</v>
       </c>
       <c r="U16" s="65">
-        <v>105.26519999999999</v>
+        <f>(1-V16)/V16</f>
+        <v>72.286918285086116</v>
       </c>
       <c r="V16" s="88">
-        <f t="shared" ref="V16" si="0">1/(1+U16)</f>
-        <v>9.4104184624881904E-3</v>
+        <v>1.3644999999999999E-2</v>
       </c>
       <c r="W16" s="65">
         <f>(1-X16)/X16</f>
@@ -33920,8 +33956,8 @@
       </c>
     </row>
     <row r="17" spans="2:32" ht="15" thickBot="1">
-      <c r="B17" s="166"/>
-      <c r="C17" s="151"/>
+      <c r="B17" s="176"/>
+      <c r="C17" s="161"/>
       <c r="D17" s="4" t="s">
         <v>70</v>
       </c>
@@ -33955,11 +33991,11 @@
         <v>1.169187E-13</v>
       </c>
       <c r="U17" s="70">
-        <v>4.3653000000000004</v>
+        <f>(1-V17)/V17</f>
+        <v>4.3682340120570533</v>
       </c>
       <c r="V17" s="89">
-        <f t="shared" ref="V17" si="1">1/(1+U17)</f>
-        <v>0.18638286768680221</v>
+        <v>0.186281</v>
       </c>
       <c r="W17" s="70">
         <f>(1-X17)/X17</f>
@@ -33972,32 +34008,32 @@
         <v>5.7611349999999997E-3</v>
       </c>
       <c r="Z17" s="70">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="70">
         <v>0</v>
-      </c>
-      <c r="AA17" s="70">
-        <v>1</v>
       </c>
       <c r="AB17" s="70">
         <v>4.7629169999999999E-14</v>
       </c>
-      <c r="AC17" s="89"/>
-      <c r="AD17" s="89"/>
-      <c r="AE17" s="89">
-        <f>(1-AF17)/AF17</f>
-        <v>4.0448996064978306</v>
-      </c>
-      <c r="AF17" s="93">
-        <v>0.19822000000000001</v>
-      </c>
+      <c r="AC17" s="89">
+        <f>(1-AD17)/AD17</f>
+        <v>57.778581085052608</v>
+      </c>
+      <c r="AD17" s="89">
+        <v>1.7013E-2</v>
+      </c>
+      <c r="AE17" s="89"/>
+      <c r="AF17" s="93"/>
     </row>
     <row r="18" spans="2:32" ht="17" thickBot="1">
-      <c r="B18" s="147" t="s">
+      <c r="B18" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="151" t="s">
+      <c r="C18" s="161" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="152"/>
+      <c r="D18" s="162"/>
       <c r="E18" s="48" t="s">
         <v>0</v>
       </c>
@@ -34084,7 +34120,7 @@
       </c>
     </row>
     <row r="19" spans="2:32" ht="15" thickBot="1">
-      <c r="B19" s="148"/>
+      <c r="B19" s="158"/>
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="34" t="s">
@@ -34125,11 +34161,11 @@
       <c r="AF19" s="56"/>
     </row>
     <row r="20" spans="2:32" ht="15" thickBot="1">
-      <c r="B20" s="149"/>
-      <c r="C20" s="160" t="s">
+      <c r="B20" s="159"/>
+      <c r="C20" s="170" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="161"/>
+      <c r="D20" s="171"/>
       <c r="E20" s="32">
         <v>1.5509999999999999E-2</v>
       </c>
@@ -34142,9 +34178,8 @@
       <c r="H20" s="50">
         <v>0</v>
       </c>
-      <c r="I20" s="50"/>
+      <c r="I20" s="57"/>
       <c r="J20" s="50">
-        <f>1/(1+I20)</f>
         <v>1</v>
       </c>
       <c r="K20" s="113"/>
@@ -34171,11 +34206,11 @@
       <c r="AF20" s="116"/>
     </row>
     <row r="21" spans="2:32" ht="15" thickBot="1">
-      <c r="B21" s="149"/>
-      <c r="C21" s="160" t="s">
+      <c r="B21" s="159"/>
+      <c r="C21" s="170" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="161"/>
+      <c r="D21" s="171"/>
       <c r="E21" s="32">
         <v>6.6889339999999997E-3</v>
       </c>
@@ -34256,7 +34291,7 @@
       </c>
     </row>
     <row r="22" spans="2:32" ht="15" thickBot="1">
-      <c r="B22" s="149"/>
+      <c r="B22" s="159"/>
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
       <c r="E22" s="34" t="s">
@@ -34297,8 +34332,8 @@
       <c r="AF22" s="56"/>
     </row>
     <row r="23" spans="2:32" ht="15" thickBot="1">
-      <c r="B23" s="149"/>
-      <c r="C23" s="162" t="s">
+      <c r="B23" s="159"/>
+      <c r="C23" s="172" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="13" t="s">
@@ -34318,10 +34353,10 @@
       </c>
       <c r="I23" s="57">
         <f>(1-J23)/J23</f>
-        <v>1</v>
+        <v>0.96261608874164917</v>
       </c>
       <c r="J23" s="83">
-        <v>0.5</v>
+        <v>0.50952399999999998</v>
       </c>
       <c r="K23" s="63">
         <v>1.651163E-3</v>
@@ -34353,8 +34388,8 @@
       <c r="AF23" s="60"/>
     </row>
     <row r="24" spans="2:32" ht="15" thickBot="1">
-      <c r="B24" s="149"/>
-      <c r="C24" s="163"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="173"/>
       <c r="D24" s="13" t="s">
         <v>67</v>
       </c>
@@ -34378,13 +34413,13 @@
         <v>0.5</v>
       </c>
       <c r="K24" s="37">
-        <v>1.651163E-3</v>
+        <v>1.9559999999999998E-3</v>
       </c>
       <c r="L24" s="57">
-        <v>0.6333974</v>
+        <v>0.62872799999999995</v>
       </c>
       <c r="M24" s="57">
-        <v>0.3666026</v>
+        <v>0.37127199999999999</v>
       </c>
       <c r="N24" s="57">
         <v>0</v>
@@ -34418,8 +34453,8 @@
       <c r="AF24" s="60"/>
     </row>
     <row r="25" spans="2:32">
-      <c r="B25" s="149"/>
-      <c r="C25" s="163"/>
+      <c r="B25" s="159"/>
+      <c r="C25" s="173"/>
       <c r="D25" s="3" t="s">
         <v>68</v>
       </c>
@@ -34440,13 +34475,13 @@
       <c r="O25" s="62"/>
       <c r="P25" s="64"/>
       <c r="Q25" s="42">
-        <v>1.4407700000000001E-2</v>
+        <v>1.3857E-2</v>
       </c>
       <c r="R25" s="65">
-        <v>0.4395963</v>
+        <v>0.44542300000000001</v>
       </c>
       <c r="S25" s="65">
-        <v>0.56040369999999995</v>
+        <v>0.55475699999999994</v>
       </c>
       <c r="T25" s="65">
         <f>8.024692*10^-13</f>
@@ -34454,29 +34489,29 @@
       </c>
       <c r="U25" s="57">
         <f>(1-V25)/V25</f>
-        <v>0.38731852139591993</v>
+        <v>105.48493238206794</v>
       </c>
       <c r="V25" s="76">
-        <v>0.72081499999999998</v>
+        <v>9.391E-3</v>
       </c>
       <c r="W25" s="57">
         <f>(1-X25)/X25</f>
-        <v>105.48493238206794</v>
+        <v>0.38731852139591993</v>
       </c>
       <c r="X25" s="85">
-        <v>9.391E-3</v>
+        <v>0.72081499999999998</v>
       </c>
       <c r="Y25" s="43">
-        <v>6.9913470000000002E-3</v>
+        <v>7.1029999999999999E-3</v>
       </c>
       <c r="Z25" s="65">
-        <v>0.42039559999999998</v>
+        <v>0.42668400000000001</v>
       </c>
       <c r="AA25" s="65">
-        <v>0.41710069999999999</v>
+        <v>0.42180400000000001</v>
       </c>
       <c r="AB25" s="65">
-        <v>0.1625037</v>
+        <v>0.15151200000000001</v>
       </c>
       <c r="AC25" s="57">
         <f>(1-AD25)/AD25</f>
@@ -34487,15 +34522,15 @@
       </c>
       <c r="AE25" s="57">
         <f>(1-AF25)/AF25</f>
-        <v>695.52434352580622</v>
+        <v>68.652434352580627</v>
       </c>
       <c r="AF25" s="85">
-        <v>1.4357E-3</v>
+        <v>1.4357E-2</v>
       </c>
     </row>
     <row r="26" spans="2:32">
-      <c r="B26" s="149"/>
-      <c r="C26" s="163"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="173"/>
       <c r="D26" s="3" t="s">
         <v>69</v>
       </c>
@@ -34516,23 +34551,23 @@
       <c r="O26" s="62"/>
       <c r="P26" s="64"/>
       <c r="Q26" s="42">
-        <v>2.2805579999999999E-2</v>
+        <v>2.0230000000000001E-2</v>
       </c>
       <c r="R26" s="65">
-        <v>0.791632</v>
+        <v>0.57004900000000003</v>
       </c>
       <c r="S26" s="65">
-        <v>2.742913E-3</v>
+        <v>0.13438700000000001</v>
       </c>
       <c r="T26" s="65">
-        <v>0.205625</v>
+        <v>0.29556399999999999</v>
       </c>
       <c r="U26" s="65">
         <f>(1-V26)/V26</f>
-        <v>13.597474636887819</v>
+        <v>1.1496685211140443</v>
       </c>
       <c r="V26" s="65">
-        <v>6.8504999999999996E-2</v>
+        <v>0.46518799999999999</v>
       </c>
       <c r="W26" s="65">
         <v>-1</v>
@@ -34541,34 +34576,33 @@
         <v>40</v>
       </c>
       <c r="Y26" s="43">
-        <v>1.3197489999999999E-2</v>
+        <v>7.1149999999999998E-3</v>
       </c>
       <c r="Z26" s="65">
-        <v>0.73795659999999996</v>
+        <v>0.469167</v>
       </c>
       <c r="AA26" s="65">
-        <v>3.4708790000000003E-2</v>
+        <v>0.14401700000000001</v>
       </c>
       <c r="AB26" s="65">
-        <v>0.2273346</v>
+        <v>0.38681700000000002</v>
       </c>
       <c r="AC26" s="65">
-        <f>(1-AD26)/AD26</f>
-        <v>8.1113682541707295</v>
-      </c>
-      <c r="AD26" s="86">
-        <v>0.109753</v>
+        <v>-1</v>
+      </c>
+      <c r="AD26" s="86" t="s">
+        <v>40</v>
       </c>
       <c r="AE26" s="65">
         <v>-1</v>
       </c>
-      <c r="AF26" s="86" t="s">
-        <v>40</v>
+      <c r="AF26" s="86">
+        <v>0.61199400000000004</v>
       </c>
     </row>
     <row r="27" spans="2:32" ht="15" thickBot="1">
-      <c r="B27" s="150"/>
-      <c r="C27" s="151"/>
+      <c r="B27" s="160"/>
+      <c r="C27" s="161"/>
       <c r="D27" s="78" t="s">
         <v>70</v>
       </c>
@@ -34589,42 +34623,42 @@
       <c r="O27" s="67"/>
       <c r="P27" s="69"/>
       <c r="Q27" s="46">
-        <v>2.2573050000000001E-2</v>
+        <v>2.2682000000000001E-2</v>
       </c>
       <c r="R27" s="70">
-        <v>0.25688480000000002</v>
+        <v>0.25429800000000002</v>
       </c>
       <c r="S27" s="70">
-        <v>0.73587780000000003</v>
+        <v>0.73824299999999998</v>
       </c>
       <c r="T27" s="70">
-        <v>7.237467E-3</v>
+        <v>7.4599999999999996E-3</v>
       </c>
       <c r="U27" s="70">
         <f>(1-V27)/V27</f>
-        <v>8.6769823298302651</v>
+        <v>-0.25401414985960546</v>
       </c>
       <c r="V27" s="70">
-        <v>0.103338</v>
+        <v>1.340508</v>
       </c>
       <c r="W27" s="70">
         <f>(1-X27)/X27</f>
-        <v>-0.25401414985960546</v>
+        <v>8.6769823298302651</v>
       </c>
       <c r="X27" s="87">
-        <v>1.340508</v>
+        <v>0.103338</v>
       </c>
       <c r="Y27" s="47">
-        <v>1.1086439999999999E-2</v>
+        <v>1.1338000000000001E-2</v>
       </c>
       <c r="Z27" s="70">
-        <v>0.30770619999999999</v>
+        <v>0.30574899999999999</v>
       </c>
       <c r="AA27" s="70">
-        <v>0.63338629999999996</v>
+        <v>0.64202199999999998</v>
       </c>
       <c r="AB27" s="70">
-        <v>5.8907550000000003E-2</v>
+        <v>5.2228999999999998E-2</v>
       </c>
       <c r="AC27" s="70">
         <f>(1-AD27)/AD27</f>
@@ -34675,19 +34709,19 @@
     </row>
     <row r="31" spans="2:32">
       <c r="F31" s="77"/>
-      <c r="G31" s="174" t="s">
+      <c r="G31" s="154" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="174"/>
-      <c r="I31" s="175"/>
-      <c r="J31" s="175"/>
-      <c r="K31" s="175"/>
-      <c r="L31" s="175"/>
-      <c r="M31" s="175"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="155"/>
+      <c r="J31" s="155"/>
+      <c r="K31" s="155"/>
+      <c r="L31" s="155"/>
+      <c r="M31" s="155"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="175"/>
-      <c r="Q31" s="175"/>
+      <c r="P31" s="155"/>
+      <c r="Q31" s="155"/>
     </row>
     <row r="32" spans="2:32">
       <c r="F32"/>
@@ -34728,16 +34762,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E6:P6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="K7:P7"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="Q6:AF6"/>
-    <mergeCell ref="Q7:X7"/>
-    <mergeCell ref="Y7:AF7"/>
     <mergeCell ref="B18:B27"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="B6:B8"/>
@@ -34749,6 +34773,16 @@
     <mergeCell ref="C23:C27"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E6:P6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="K7:P7"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="Q6:AF6"/>
+    <mergeCell ref="Q7:X7"/>
+    <mergeCell ref="Y7:AF7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="landscape"/>
@@ -34765,7 +34799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -35146,11 +35180,11 @@
       </c>
       <c r="G45" s="120">
         <f t="shared" si="5"/>
-        <v>8.1543252615262712E-2</v>
+        <v>8.5312692500270279E-2</v>
       </c>
       <c r="H45" s="120">
         <f t="shared" ref="H45:H47" si="7">SUM(D45:G45)</f>
-        <v>0.99999998246650934</v>
+        <v>1.0037694223515168</v>
       </c>
       <c r="I45" s="97">
         <f>'Results Table'!Y15</f>
@@ -35166,7 +35200,7 @@
       </c>
       <c r="L45" s="97">
         <f>'Results Table'!AB15</f>
-        <v>9.2871880000000004E-2</v>
+        <v>9.7165000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="2:12">
@@ -35220,11 +35254,11 @@
       </c>
       <c r="E47" s="120">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.84429364864864864</v>
       </c>
       <c r="F47" s="120">
         <f t="shared" si="5"/>
-        <v>0.84429364864864864</v>
+        <v>0</v>
       </c>
       <c r="G47" s="120">
         <f t="shared" si="5"/>
@@ -35240,11 +35274,11 @@
       </c>
       <c r="J47" s="97">
         <f>'Results Table'!Z17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" s="97">
         <f>'Results Table'!AA17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="97">
         <f>'Results Table'!AB17</f>
@@ -35414,35 +35448,35 @@
       </c>
       <c r="D55" s="122">
         <f t="shared" si="8"/>
-        <v>0.6003208333333333</v>
+        <v>0.57737499999999997</v>
       </c>
       <c r="E55" s="120">
         <f t="shared" si="9"/>
-        <v>0.17569748285375</v>
+        <v>0.18824689537500003</v>
       </c>
       <c r="F55" s="120">
         <f t="shared" si="9"/>
-        <v>0.22398168381291667</v>
+        <v>0.234454177125</v>
       </c>
       <c r="G55" s="120">
         <f t="shared" si="9"/>
-        <v>3.2073022113166671E-13</v>
+        <v>3.3914354565000002E-13</v>
       </c>
       <c r="H55" s="120">
         <f t="shared" ref="H55:H57" si="14">SUM(D55:G55)</f>
-        <v>1.0000000000003206</v>
+        <v>1.000076072500339</v>
       </c>
       <c r="I55" s="121">
         <f>'Results Table'!Q25</f>
-        <v>1.4407700000000001E-2</v>
+        <v>1.3857E-2</v>
       </c>
       <c r="J55" s="121">
         <f>'Results Table'!R25</f>
-        <v>0.4395963</v>
+        <v>0.44542300000000001</v>
       </c>
       <c r="K55" s="121">
         <f>'Results Table'!S25</f>
-        <v>0.56040369999999995</v>
+        <v>0.55475699999999994</v>
       </c>
       <c r="L55" s="121">
         <f>'Results Table'!T25</f>
@@ -35455,39 +35489,39 @@
       </c>
       <c r="D56" s="120">
         <f t="shared" si="8"/>
-        <v>0.95023249999999992</v>
+        <v>0.84291666666666676</v>
       </c>
       <c r="E56" s="120">
         <f t="shared" si="9"/>
-        <v>3.9397545560000059E-2</v>
+        <v>8.9545197083333292E-2</v>
       </c>
       <c r="F56" s="120">
         <f t="shared" si="9"/>
-        <v>1.3650792272750021E-4</v>
+        <v>2.1109957916666654E-2</v>
       </c>
       <c r="G56" s="120">
         <f t="shared" si="9"/>
-        <v>1.0233442187500016E-2</v>
+        <v>4.6428178333333306E-2</v>
       </c>
       <c r="H56" s="120">
         <f t="shared" si="14"/>
-        <v>0.99999999567022746</v>
+        <v>1</v>
       </c>
       <c r="I56" s="121">
         <f>'Results Table'!Q26</f>
-        <v>2.2805579999999999E-2</v>
+        <v>2.0230000000000001E-2</v>
       </c>
       <c r="J56" s="121">
         <f>'Results Table'!R26</f>
-        <v>0.791632</v>
+        <v>0.57004900000000003</v>
       </c>
       <c r="K56" s="121">
         <f>'Results Table'!S26</f>
-        <v>2.742913E-3</v>
+        <v>0.13438700000000001</v>
       </c>
       <c r="L56" s="121">
         <f>'Results Table'!T26</f>
-        <v>0.205625</v>
+        <v>0.29556399999999999</v>
       </c>
     </row>
     <row r="57" spans="2:12">
@@ -35496,39 +35530,39 @@
       </c>
       <c r="D57" s="120">
         <f t="shared" si="8"/>
-        <v>0.94054375000000001</v>
+        <v>0.94508333333333339</v>
       </c>
       <c r="E57" s="120">
         <f t="shared" si="9"/>
-        <v>1.5273406889999999E-2</v>
+        <v>1.3965198499999987E-2</v>
       </c>
       <c r="F57" s="120">
         <f t="shared" si="9"/>
-        <v>4.3752534446249991E-2</v>
+        <v>4.0541844749999958E-2</v>
       </c>
       <c r="G57" s="120">
         <f t="shared" si="9"/>
-        <v>4.3031264731874989E-4</v>
+        <v>4.096783333333329E-4</v>
       </c>
       <c r="H57" s="120">
         <f t="shared" si="14"/>
-        <v>1.0000000039835688</v>
+        <v>1.0000000549166668</v>
       </c>
       <c r="I57" s="121">
         <f>'Results Table'!Q27</f>
-        <v>2.2573050000000001E-2</v>
+        <v>2.2682000000000001E-2</v>
       </c>
       <c r="J57" s="121">
         <f>'Results Table'!R27</f>
-        <v>0.25688480000000002</v>
+        <v>0.25429800000000002</v>
       </c>
       <c r="K57" s="121">
         <f>'Results Table'!S27</f>
-        <v>0.73587780000000003</v>
+        <v>0.73824299999999998</v>
       </c>
       <c r="L57" s="121">
         <f>'Results Table'!T27</f>
-        <v>7.237467E-3</v>
+        <v>7.4599999999999996E-3</v>
       </c>
     </row>
     <row r="58" spans="2:12">
@@ -35537,15 +35571,15 @@
       </c>
       <c r="D58" s="120">
         <f t="shared" si="8"/>
-        <v>6.8798458333333326E-2</v>
+        <v>8.1499999999999989E-2</v>
       </c>
       <c r="E58" s="120">
         <f t="shared" si="9"/>
-        <v>0.58982063536765839</v>
+        <v>0.57748666799999993</v>
       </c>
       <c r="F58" s="120">
         <f t="shared" si="9"/>
-        <v>0.34138090629900836</v>
+        <v>0.341013332</v>
       </c>
       <c r="G58" s="120">
         <f t="shared" si="9"/>
@@ -35557,15 +35591,15 @@
       </c>
       <c r="I58" s="121">
         <f>'Results Table'!K24</f>
-        <v>1.651163E-3</v>
+        <v>1.9559999999999998E-3</v>
       </c>
       <c r="J58" s="121">
         <f>'Results Table'!L24</f>
-        <v>0.6333974</v>
+        <v>0.62872799999999995</v>
       </c>
       <c r="K58" s="121">
         <f>'Results Table'!M24</f>
-        <v>0.3666026</v>
+        <v>0.37127199999999999</v>
       </c>
       <c r="L58" s="121">
         <f>'Results Table'!N23</f>
@@ -35578,19 +35612,19 @@
       </c>
       <c r="D59" s="122">
         <f t="shared" si="8"/>
-        <v>0.29130612500000003</v>
+        <v>0.29595833333333332</v>
       </c>
       <c r="E59" s="120">
         <f t="shared" si="9"/>
-        <v>0.29793178679694998</v>
+        <v>0.30040331450000002</v>
       </c>
       <c r="F59" s="120">
         <f t="shared" si="9"/>
-        <v>0.29559671134821253</v>
+        <v>0.29696759116666666</v>
       </c>
       <c r="G59" s="120">
         <f t="shared" si="9"/>
-        <v>0.11516537685483751</v>
+        <v>0.106670761</v>
       </c>
       <c r="H59" s="120">
         <f t="shared" ref="H59:H61" si="15">SUM(D59:G59)</f>
@@ -35598,19 +35632,19 @@
       </c>
       <c r="I59" s="121">
         <f>'Results Table'!Y25</f>
-        <v>6.9913470000000002E-3</v>
+        <v>7.1029999999999999E-3</v>
       </c>
       <c r="J59" s="121">
         <f>'Results Table'!Z25</f>
-        <v>0.42039559999999998</v>
+        <v>0.42668400000000001</v>
       </c>
       <c r="K59" s="121">
         <f>'Results Table'!AA25</f>
-        <v>0.41710069999999999</v>
+        <v>0.42180400000000001</v>
       </c>
       <c r="L59" s="121">
         <f>'Results Table'!AB25</f>
-        <v>0.1625037</v>
+        <v>0.15151200000000001</v>
       </c>
     </row>
     <row r="60" spans="2:12">
@@ -35619,39 +35653,39 @@
       </c>
       <c r="D60" s="120">
         <f t="shared" si="8"/>
-        <v>0.54989541666666664</v>
+        <v>0.29645833333333332</v>
       </c>
       <c r="E60" s="120">
         <f t="shared" si="9"/>
-        <v>0.33215764796108332</v>
+        <v>0.33007853312500002</v>
       </c>
       <c r="F60" s="120">
         <f t="shared" si="9"/>
-        <v>1.5622585460954169E-2</v>
+        <v>0.10132196020833335</v>
       </c>
       <c r="G60" s="120">
         <f t="shared" si="9"/>
-        <v>0.10232434541025001</v>
+        <v>0.27214187687500002</v>
       </c>
       <c r="H60" s="120">
         <f t="shared" si="15"/>
-        <v>0.99999999549895424</v>
+        <v>1.0000007035416667</v>
       </c>
       <c r="I60" s="121">
         <f>'Results Table'!Y26</f>
-        <v>1.3197489999999999E-2</v>
+        <v>7.1149999999999998E-3</v>
       </c>
       <c r="J60" s="121">
         <f>'Results Table'!Z26</f>
-        <v>0.73795659999999996</v>
+        <v>0.469167</v>
       </c>
       <c r="K60" s="121">
         <f>'Results Table'!AA26</f>
-        <v>3.4708790000000003E-2</v>
+        <v>0.14401700000000001</v>
       </c>
       <c r="L60" s="121">
         <f>'Results Table'!AB26</f>
-        <v>0.2273346</v>
+        <v>0.38681700000000002</v>
       </c>
     </row>
     <row r="61" spans="2:12">
@@ -35660,39 +35694,39 @@
       </c>
       <c r="D61" s="120">
         <f t="shared" si="8"/>
-        <v>0.46193499999999998</v>
+        <v>0.47241666666666671</v>
       </c>
       <c r="E61" s="120">
         <f t="shared" si="9"/>
-        <v>0.165565936503</v>
+        <v>0.16130807658333332</v>
       </c>
       <c r="F61" s="120">
         <f t="shared" si="9"/>
-        <v>0.34080299950949999</v>
+        <v>0.33872010683333331</v>
       </c>
       <c r="G61" s="120">
         <f t="shared" si="9"/>
-        <v>3.1696090890750005E-2</v>
+        <v>2.7555149916666664E-2</v>
       </c>
       <c r="H61" s="120">
         <f t="shared" si="15"/>
-        <v>1.0000000269032501</v>
+        <v>1</v>
       </c>
       <c r="I61" s="121">
         <f>'Results Table'!Y27</f>
-        <v>1.1086439999999999E-2</v>
+        <v>1.1338000000000001E-2</v>
       </c>
       <c r="J61" s="121">
         <f>'Results Table'!Z27</f>
-        <v>0.30770619999999999</v>
+        <v>0.30574899999999999</v>
       </c>
       <c r="K61" s="121">
         <f>'Results Table'!AA27</f>
-        <v>0.63338629999999996</v>
+        <v>0.64202199999999998</v>
       </c>
       <c r="L61" s="121">
         <f>'Results Table'!AB27</f>
-        <v>5.8907550000000003E-2</v>
+        <v>5.2228999999999998E-2</v>
       </c>
     </row>
     <row r="62" spans="2:12">
@@ -35740,11 +35774,11 @@
       </c>
       <c r="E69" s="79">
         <f t="shared" ref="E69:G69" si="16">E47*$B$3</f>
-        <v>0</v>
+        <v>3.1238864999999998E-2</v>
       </c>
       <c r="F69" s="79">
         <f t="shared" si="16"/>
-        <v>3.1238864999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="G69" s="79">
         <f t="shared" si="16"/>
@@ -35800,11 +35834,11 @@
       </c>
       <c r="G71" s="79">
         <f t="shared" si="18"/>
-        <v>3.0171003467647202E-3</v>
+        <v>3.1565696225100003E-3</v>
       </c>
       <c r="H71" s="80">
         <f>SUM(D71:G71)</f>
-        <v>3.6999999351260845E-2</v>
+        <v>3.7139468627006123E-2</v>
       </c>
     </row>
     <row r="72" spans="2:8">
@@ -36010,23 +36044,23 @@
       </c>
       <c r="D83" s="127">
         <f>D61*$C$3</f>
-        <v>1.1086439999999999E-2</v>
+        <v>1.1338000000000001E-2</v>
       </c>
       <c r="E83" s="127">
         <f t="shared" ref="E83:G83" si="27">E61*$C$3</f>
-        <v>3.9735824760720002E-3</v>
+        <v>3.8713938379999996E-3</v>
       </c>
       <c r="F83" s="127">
         <f t="shared" si="27"/>
-        <v>8.1792719882279995E-3</v>
+        <v>8.1292825639999993E-3</v>
       </c>
       <c r="G83" s="127">
         <f t="shared" si="27"/>
-        <v>7.6070618137800017E-4</v>
+        <v>6.613235979999999E-4</v>
       </c>
       <c r="H83" s="120">
         <f>SUM(D83:G83)</f>
-        <v>2.4000000645678001E-2</v>
+        <v>2.3999999999999997E-2</v>
       </c>
     </row>
     <row r="84" spans="3:9">
@@ -36036,23 +36070,23 @@
       </c>
       <c r="D84" s="127">
         <f>D60*$C$3</f>
-        <v>1.3197489999999999E-2</v>
+        <v>7.1149999999999998E-3</v>
       </c>
       <c r="E84" s="127">
         <f t="shared" ref="E84:G84" si="28">E60*$C$3</f>
-        <v>7.9717835510659998E-3</v>
+        <v>7.9218847950000004E-3</v>
       </c>
       <c r="F84" s="127">
         <f t="shared" si="28"/>
-        <v>3.7494205106290007E-4</v>
+        <v>2.4317270450000005E-3</v>
       </c>
       <c r="G84" s="127">
         <f t="shared" si="28"/>
-        <v>2.4557842898460004E-3</v>
+        <v>6.5314050450000008E-3</v>
       </c>
       <c r="H84" s="120">
         <f>SUM(D84:G84)</f>
-        <v>2.3999999891974901E-2</v>
+        <v>2.4000016885000003E-2</v>
       </c>
     </row>
     <row r="85" spans="3:9">
@@ -36062,19 +36096,19 @@
       </c>
       <c r="D85" s="127">
         <f>D59*$C$3</f>
-        <v>6.9913470000000011E-3</v>
+        <v>7.1029999999999999E-3</v>
       </c>
       <c r="E85" s="127">
         <f t="shared" ref="E85:G85" si="29">E59*$C$3</f>
-        <v>7.1503628831267995E-3</v>
+        <v>7.2096795480000005E-3</v>
       </c>
       <c r="F85" s="127">
         <f t="shared" si="29"/>
-        <v>7.094321072357101E-3</v>
+        <v>7.127222188E-3</v>
       </c>
       <c r="G85" s="127">
         <f t="shared" si="29"/>
-        <v>2.7639690445161002E-3</v>
+        <v>2.560098264E-3</v>
       </c>
       <c r="H85" s="120">
         <f t="shared" ref="H85:H87" si="30">SUM(D85:G85)</f>
@@ -36088,15 +36122,15 @@
       </c>
       <c r="D86" s="127">
         <f>D58*$C$3</f>
-        <v>1.6511629999999998E-3</v>
+        <v>1.9559999999999998E-3</v>
       </c>
       <c r="E86" s="127">
         <f t="shared" ref="E86:G86" si="31">E58*$C$3</f>
-        <v>1.4155695248823801E-2</v>
+        <v>1.3859680031999999E-2</v>
       </c>
       <c r="F86" s="127">
         <f t="shared" si="31"/>
-        <v>8.1931417511762004E-3</v>
+        <v>8.1843199680000003E-3</v>
       </c>
       <c r="G86" s="127">
         <f t="shared" si="31"/>
@@ -36114,23 +36148,23 @@
       </c>
       <c r="D87" s="127">
         <f>D57*$C$3</f>
-        <v>2.2573050000000001E-2</v>
+        <v>2.2682000000000001E-2</v>
       </c>
       <c r="E87" s="127">
         <f t="shared" ref="E87:G87" si="32">E57*$C$3</f>
-        <v>3.6656176535999999E-4</v>
+        <v>3.351647639999997E-4</v>
       </c>
       <c r="F87" s="127">
         <f t="shared" si="32"/>
-        <v>1.0500608267099997E-3</v>
+        <v>9.7300427399999898E-4</v>
       </c>
       <c r="G87" s="127">
         <f t="shared" si="32"/>
-        <v>1.0327503535649997E-5</v>
+        <v>9.8322799999999891E-6</v>
       </c>
       <c r="H87" s="120">
         <f t="shared" si="30"/>
-        <v>2.4000000095605652E-2</v>
+        <v>2.4000001318000001E-2</v>
       </c>
     </row>
     <row r="88" spans="3:9">
@@ -36140,23 +36174,23 @@
       </c>
       <c r="D88" s="127">
         <f>D56*$C$3</f>
-        <v>2.2805579999999999E-2</v>
+        <v>2.0230000000000001E-2</v>
       </c>
       <c r="E88" s="127">
         <f t="shared" ref="E88:G88" si="33">E56*$C$3</f>
-        <v>9.4554109344000144E-4</v>
+        <v>2.1490847299999991E-3</v>
       </c>
       <c r="F88" s="127">
         <f t="shared" si="33"/>
-        <v>3.2761901454600052E-6</v>
+        <v>5.0663898999999974E-4</v>
       </c>
       <c r="G88" s="127">
         <f t="shared" si="33"/>
-        <v>2.4560261250000041E-4</v>
+        <v>1.1142762799999993E-3</v>
       </c>
       <c r="H88" s="120">
         <f>SUM(D88:G88)</f>
-        <v>2.3999999896085457E-2</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="89" spans="3:9">
@@ -36166,23 +36200,23 @@
       </c>
       <c r="D89" s="127">
         <f>D55*$C$3</f>
-        <v>1.4407699999999999E-2</v>
+        <v>1.3857E-2</v>
       </c>
       <c r="E89" s="127">
         <f t="shared" ref="E89:G89" si="34">E55*$C$3</f>
-        <v>4.2167395884900004E-3</v>
+        <v>4.517925489000001E-3</v>
       </c>
       <c r="F89" s="127">
         <f t="shared" si="34"/>
-        <v>5.3755604115100003E-3</v>
+        <v>5.6269002510000001E-3</v>
       </c>
       <c r="G89" s="127">
         <f t="shared" si="34"/>
-        <v>7.6975253071600017E-15</v>
+        <v>8.1394450956E-15</v>
       </c>
       <c r="H89" s="120">
         <f t="shared" ref="H89:H91" si="35">SUM(D89:G89)</f>
-        <v>2.4000000000007699E-2</v>
+        <v>2.4001825740008139E-2</v>
       </c>
     </row>
     <row r="90" spans="3:9">
@@ -36280,7 +36314,7 @@
       </c>
       <c r="D95" s="107">
         <f>'Results Table'!V15</f>
-        <v>1.9770660340055357</v>
+        <v>1.74712</v>
       </c>
       <c r="E95" s="65">
         <f>'Results Table'!X15</f>
@@ -36299,7 +36333,7 @@
       <c r="E96" s="108"/>
       <c r="F96" s="65">
         <f>'Results Table'!V16</f>
-        <v>9.4104184624881904E-3</v>
+        <v>1.3644999999999999E-2</v>
       </c>
       <c r="G96" s="65">
         <f>'Results Table'!X16</f>
@@ -36318,7 +36352,7 @@
       <c r="G97" s="112"/>
       <c r="H97" s="70">
         <f>'Results Table'!V17</f>
-        <v>0.18638286768680221</v>
+        <v>0.186281</v>
       </c>
       <c r="I97" s="71">
         <f>'Results Table'!X17</f>
@@ -36397,7 +36431,7 @@
       <c r="H102" s="70"/>
       <c r="I102" s="71">
         <f>'Results Table'!AF17</f>
-        <v>0.19822000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="3:9" ht="15" thickBot="1"/>
@@ -36443,7 +36477,7 @@
       </c>
       <c r="D107" s="107">
         <f>'Results Table'!J23</f>
-        <v>0.5</v>
+        <v>0.50952399999999998</v>
       </c>
       <c r="E107" s="108"/>
       <c r="F107" s="108"/>
@@ -36457,11 +36491,11 @@
       </c>
       <c r="D108" s="107">
         <f>'Results Table'!V25</f>
-        <v>0.72081499999999998</v>
+        <v>9.391E-3</v>
       </c>
       <c r="E108" s="65">
         <f>'Results Table'!X25</f>
-        <v>9.391E-3</v>
+        <v>0.72081499999999998</v>
       </c>
       <c r="F108" s="108"/>
       <c r="G108" s="108"/>
@@ -36476,7 +36510,7 @@
       <c r="E109" s="108"/>
       <c r="F109" s="65">
         <f>'Results Table'!V26</f>
-        <v>6.8504999999999996E-2</v>
+        <v>0.46518799999999999</v>
       </c>
       <c r="G109" s="65" t="str">
         <f>'Results Table'!X26</f>
@@ -36495,11 +36529,11 @@
       <c r="G110" s="112"/>
       <c r="H110" s="70">
         <f>'Results Table'!V27</f>
-        <v>0.103338</v>
+        <v>1.340508</v>
       </c>
       <c r="I110" s="71">
         <f>'Results Table'!X27</f>
-        <v>1.340508</v>
+        <v>0.103338</v>
       </c>
     </row>
     <row r="111" spans="3:9">
@@ -36539,7 +36573,7 @@
       </c>
       <c r="E113" s="65">
         <f>'Results Table'!AF25</f>
-        <v>1.4357E-3</v>
+        <v>1.4357E-2</v>
       </c>
       <c r="F113" s="108"/>
       <c r="G113" s="108"/>
@@ -36552,13 +36586,13 @@
       </c>
       <c r="D114" s="110"/>
       <c r="E114" s="108"/>
-      <c r="F114" s="65">
+      <c r="F114" s="65" t="str">
         <f>'Results Table'!AD26</f>
-        <v>0.109753</v>
-      </c>
-      <c r="G114" s="65" t="str">
+        <v>INF</v>
+      </c>
+      <c r="G114" s="65">
         <f>'Results Table'!AF26</f>
-        <v>INF</v>
+        <v>0.61199400000000004</v>
       </c>
       <c r="H114" s="108"/>
       <c r="I114" s="109"/>
@@ -36635,7 +36669,7 @@
       </c>
       <c r="D121" s="136">
         <f>D95</f>
-        <v>1.9770660340055357</v>
+        <v>1.74712</v>
       </c>
       <c r="E121" s="135">
         <f>E95</f>
@@ -36685,7 +36719,7 @@
       </c>
       <c r="D124" s="136">
         <f>D107</f>
-        <v>0.5</v>
+        <v>0.50952399999999998</v>
       </c>
       <c r="E124" s="139"/>
       <c r="F124" s="80"/>
@@ -36699,11 +36733,11 @@
       </c>
       <c r="D125" s="136">
         <f>D108</f>
-        <v>0.72081499999999998</v>
+        <v>9.391E-3</v>
       </c>
       <c r="E125" s="135">
         <f>E108</f>
-        <v>9.391E-3</v>
+        <v>0.72081499999999998</v>
       </c>
       <c r="F125" s="80"/>
       <c r="G125" s="80"/>
@@ -36720,7 +36754,7 @@
       </c>
       <c r="E126" s="137">
         <f>E113</f>
-        <v>1.4357E-3</v>
+        <v>1.4357E-2</v>
       </c>
       <c r="F126" s="80"/>
       <c r="G126" s="80"/>

</xml_diff>